<commit_message>
set game selection taskObject based on task
</commit_message>
<xml_diff>
--- a/Deliverable_4/Blackbear-Consultants_Deliverable_4_SprintBacklog_6.xlsx
+++ b/Deliverable_4/Blackbear-Consultants_Deliverable_4_SprintBacklog_6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\Documents\GitHub\Blackbear-Consultants\Deliverable_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Desktop/Blackbear-Consultants-Git/Deliverable_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB70D1E-4374-4D3D-A1E1-D608538091FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC501E7-890B-A04A-A4EF-76C1C3D382B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{29D05152-AD15-448E-8A0D-C19F810C4EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="D1-Sprint 1" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="D3-Sprint 5" sheetId="6" r:id="rId5"/>
     <sheet name="D4-Sprint 6" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -564,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -761,6 +761,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,24 +1084,24 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" customWidth="1"/>
-    <col min="2" max="2" width="95.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" customWidth="1"/>
+    <col min="2" max="2" width="95.33203125" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="9.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="9.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="D3" s="10"/>
@@ -1181,7 +1183,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="D4" s="10"/>
@@ -1193,7 +1195,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="D5" s="10"/>
@@ -1205,7 +1207,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="D6" s="10"/>
@@ -1217,7 +1219,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="D7" s="10"/>
@@ -1229,7 +1231,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="D8" s="10"/>
@@ -1247,7 +1249,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="23"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1262,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -1277,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1292,7 +1294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1305,15 +1307,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
     </row>
@@ -1330,25 +1332,25 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" customWidth="1"/>
-    <col min="2" max="2" width="95.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" customWidth="1"/>
+    <col min="2" max="2" width="95.33203125" customWidth="1"/>
     <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="9.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="9.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1385,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>29</v>
       </c>
@@ -1418,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="12"/>
       <c r="D3" s="10"/>
@@ -1430,7 +1432,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
       <c r="B4" s="12"/>
       <c r="D4" s="10"/>
@@ -1442,7 +1444,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="12"/>
       <c r="D5" s="10"/>
@@ -1454,7 +1456,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="12"/>
       <c r="D6" s="10"/>
@@ -1466,7 +1468,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="12"/>
       <c r="D7" s="10"/>
@@ -1478,7 +1480,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="12"/>
       <c r="D8" s="10"/>
@@ -1496,7 +1498,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1511,7 +1513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -1526,7 +1528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1541,7 +1543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1554,15 +1556,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="M15" s="2"/>
       <c r="N15" s="6"/>
     </row>
@@ -1580,23 +1582,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
+    <col min="2" max="2" width="52.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>30</v>
       </c>
@@ -1666,37 +1668,37 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="12"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
       <c r="B4" s="12"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="12"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="12"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="12"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="12"/>
       <c r="C8" s="10"/>
@@ -1706,7 +1708,7 @@
       </c>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="M9" s="6" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="M10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="M11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1730,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="M12" s="6"/>
       <c r="N12" s="6" t="s">
         <v>10</v>
@@ -1750,17 +1752,17 @@
       <selection activeCell="B10" sqref="B10:M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="44.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>35</v>
       </c>
@@ -1803,7 +1805,7 @@
       <c r="N1" s="29"/>
       <c r="O1" s="29"/>
     </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>23</v>
       </c>
@@ -1846,7 +1848,7 @@
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
     </row>
-    <row r="3" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="33" t="s">
         <v>25</v>
@@ -1887,7 +1889,7 @@
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
     </row>
-    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="B4" s="31" t="s">
         <v>21</v>
@@ -1928,7 +1930,7 @@
       <c r="N4" s="29"/>
       <c r="O4" s="29"/>
     </row>
-    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="B5" s="34" t="s">
         <v>26</v>
@@ -1969,7 +1971,7 @@
       <c r="N5" s="29"/>
       <c r="O5" s="29"/>
     </row>
-    <row r="6" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="31" t="s">
         <v>27</v>
@@ -2010,7 +2012,7 @@
       <c r="N6" s="29"/>
       <c r="O6" s="29"/>
     </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="42" t="s">
         <v>32</v>
@@ -2051,7 +2053,7 @@
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
     </row>
-    <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="42" t="s">
         <v>38</v>
@@ -2092,7 +2094,7 @@
       <c r="N8" s="29"/>
       <c r="O8" s="29"/>
     </row>
-    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="31" t="s">
         <v>39</v>
@@ -2133,7 +2135,7 @@
       <c r="N9" s="29"/>
       <c r="O9" s="29"/>
     </row>
-    <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="42" t="s">
         <v>40</v>
@@ -2174,7 +2176,7 @@
       <c r="N10" s="29"/>
       <c r="O10" s="29"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
@@ -2193,7 +2195,7 @@
       </c>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2214,7 +2216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -2235,7 +2237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -2256,7 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -2284,27 +2286,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E667C8-1B91-474D-8867-5FDB69B5DA40}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>34</v>
       </c>
@@ -2347,7 +2349,7 @@
       <c r="N1" s="29"/>
       <c r="O1" s="29"/>
     </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>31</v>
       </c>
@@ -2390,7 +2392,7 @@
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
     </row>
-    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="42" t="s">
         <v>21</v>
@@ -2431,7 +2433,7 @@
       <c r="N3" s="29"/>
       <c r="O3" s="29"/>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="B4" s="42" t="s">
         <v>32</v>
@@ -2472,7 +2474,7 @@
       <c r="N4" s="29"/>
       <c r="O4" s="29"/>
     </row>
-    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="B5" s="42" t="s">
         <v>33</v>
@@ -2513,24 +2515,38 @@
       <c r="N5" s="29"/>
       <c r="O5" s="29"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
+      <c r="G6" s="90">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H6" s="90">
+        <v>0.15</v>
+      </c>
+      <c r="I6" s="29">
+        <v>42.5</v>
+      </c>
+      <c r="J6" s="90">
+        <v>0.05</v>
+      </c>
+      <c r="K6" s="91">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="L6" s="90">
+        <v>0</v>
+      </c>
+      <c r="M6" s="90">
+        <v>0.05</v>
+      </c>
       <c r="N6" s="29"/>
       <c r="O6" s="29"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
@@ -2547,7 +2563,7 @@
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
@@ -2564,7 +2580,7 @@
       <c r="N8" s="29"/>
       <c r="O8" s="29"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
@@ -2581,7 +2597,7 @@
       <c r="N9" s="29"/>
       <c r="O9" s="29"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -2598,7 +2614,7 @@
       <c r="N10" s="29"/>
       <c r="O10" s="29"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
@@ -2617,7 +2633,7 @@
       </c>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="29"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2638,7 +2654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -2659,7 +2675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -2680,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -2708,31 +2724,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D424B6-0A2D-4B8E-A00A-7527EDEF6888}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="55" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="55"/>
-    <col min="6" max="6" width="12.140625" style="55" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="55" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="55" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="55" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="55"/>
+    <col min="6" max="6" width="12.1640625" style="55" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="55" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="55" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="55" customWidth="1"/>
     <col min="10" max="10" width="17" style="55" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="55" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="55" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="55" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" style="55" customWidth="1"/>
-    <col min="15" max="15" width="27.140625" style="55" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="55"/>
+    <col min="11" max="11" width="15.1640625" style="55" customWidth="1"/>
+    <col min="12" max="12" width="14.5" style="55" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="55" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" style="55" customWidth="1"/>
+    <col min="15" max="15" width="27.1640625" style="55" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
         <v>41</v>
       </c>
@@ -2775,7 +2791,7 @@
       <c r="N1" s="54"/>
       <c r="O1" s="54"/>
     </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="56" t="s">
         <v>42</v>
       </c>
@@ -2786,7 +2802,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="60" t="s">
         <v>22</v>
@@ -2818,7 +2834,7 @@
       <c r="N2" s="54"/>
       <c r="O2" s="54"/>
     </row>
-    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="54"/>
       <c r="B3" s="62" t="s">
         <v>21</v>
@@ -2827,7 +2843,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="59">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="60" t="s">
         <v>22</v>
@@ -2859,7 +2875,7 @@
       <c r="N3" s="54"/>
       <c r="O3" s="54"/>
     </row>
-    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="54"/>
       <c r="B4" s="63" t="s">
         <v>27</v>
@@ -2868,13 +2884,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="64">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="60" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="61">
         <v>0.1</v>
@@ -2900,7 +2916,7 @@
       <c r="N4" s="54"/>
       <c r="O4" s="54"/>
     </row>
-    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="54"/>
       <c r="B5" s="62" t="s">
         <v>38</v>
@@ -2909,13 +2925,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="60" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="61">
         <v>0.1</v>
@@ -2941,7 +2957,7 @@
       <c r="N5" s="54"/>
       <c r="O5" s="54"/>
     </row>
-    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="54"/>
       <c r="B6" s="63" t="s">
         <v>39</v>
@@ -2950,13 +2966,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="60">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="60" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6" s="61">
         <v>0.1</v>
@@ -2982,7 +2998,7 @@
       <c r="N6" s="54"/>
       <c r="O6" s="54"/>
     </row>
-    <row r="7" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="65"/>
       <c r="B7" s="75" t="s">
         <v>44</v>
@@ -3001,7 +3017,7 @@
       <c r="N7" s="65"/>
       <c r="O7" s="65"/>
     </row>
-    <row r="8" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="65"/>
       <c r="B8" s="76" t="s">
         <v>45</v>
@@ -3020,7 +3036,7 @@
       <c r="N8" s="65"/>
       <c r="O8" s="65"/>
     </row>
-    <row r="9" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="65"/>
       <c r="B9" s="75" t="s">
         <v>46</v>
@@ -3039,7 +3055,7 @@
       <c r="N9" s="65"/>
       <c r="O9" s="65"/>
     </row>
-    <row r="10" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="65"/>
       <c r="B10" s="66" t="s">
         <v>47</v>
@@ -3058,7 +3074,7 @@
       <c r="N10" s="65"/>
       <c r="O10" s="65"/>
     </row>
-    <row r="11" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="65"/>
       <c r="B11" s="76" t="s">
         <v>48</v>
@@ -3077,7 +3093,7 @@
       <c r="N11" s="65"/>
       <c r="O11" s="65"/>
     </row>
-    <row r="12" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="65"/>
       <c r="B12" s="76" t="s">
         <v>51</v>
@@ -3096,7 +3112,7 @@
       <c r="N12" s="65"/>
       <c r="O12" s="65"/>
     </row>
-    <row r="13" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="65"/>
       <c r="B13" s="76" t="s">
         <v>56</v>
@@ -3115,7 +3131,7 @@
       <c r="N13" s="65"/>
       <c r="O13" s="65"/>
     </row>
-    <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
       <c r="B14" s="62" t="s">
         <v>40</v>
@@ -3124,13 +3140,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="60">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E14" s="60" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G14" s="61">
         <v>0.1</v>
@@ -3156,7 +3172,7 @@
       <c r="N14" s="51"/>
       <c r="O14" s="51"/>
     </row>
-    <row r="15" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
       <c r="B15" s="62" t="s">
         <v>33</v>
@@ -3165,7 +3181,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="59">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="60" t="s">
         <v>22</v>
@@ -3197,7 +3213,7 @@
       <c r="N15" s="54"/>
       <c r="O15" s="54"/>
     </row>
-    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
       <c r="B16" s="63" t="s">
         <v>24</v>
@@ -3206,13 +3222,13 @@
         <v>4</v>
       </c>
       <c r="D16" s="64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="60" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G16" s="61">
         <v>0.1</v>
@@ -3238,7 +3254,7 @@
       <c r="N16" s="54"/>
       <c r="O16" s="54"/>
     </row>
-    <row r="17" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="65"/>
       <c r="B17" s="66" t="s">
         <v>43</v>
@@ -3257,7 +3273,7 @@
       <c r="N17" s="65"/>
       <c r="O17" s="65"/>
     </row>
-    <row r="18" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="65"/>
       <c r="B18" s="76" t="s">
         <v>52</v>
@@ -3276,7 +3292,7 @@
       <c r="N18" s="65"/>
       <c r="O18" s="65"/>
     </row>
-    <row r="19" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="65"/>
       <c r="B19" s="76" t="s">
         <v>55</v>
@@ -3295,7 +3311,7 @@
       <c r="N19" s="65"/>
       <c r="O19" s="65"/>
     </row>
-    <row r="20" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="B20" s="72" t="s">
         <v>25</v>
@@ -3304,13 +3320,13 @@
         <v>4</v>
       </c>
       <c r="D20" s="73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="60" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="60">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G20" s="61">
         <v>0.1</v>
@@ -3336,7 +3352,7 @@
       <c r="N20" s="54"/>
       <c r="O20" s="54"/>
     </row>
-    <row r="21" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="B21" s="62" t="s">
         <v>32</v>
@@ -3345,7 +3361,7 @@
         <v>4</v>
       </c>
       <c r="D21" s="59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="60" t="s">
         <v>22</v>
@@ -3377,7 +3393,7 @@
       <c r="N21" s="54"/>
       <c r="O21" s="54"/>
     </row>
-    <row r="22" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="65"/>
       <c r="B22" s="76" t="s">
         <v>49</v>
@@ -3396,7 +3412,7 @@
       <c r="N22" s="65"/>
       <c r="O22" s="65"/>
     </row>
-    <row r="23" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="65"/>
       <c r="B23" s="76" t="s">
         <v>50</v>
@@ -3415,7 +3431,7 @@
       <c r="N23" s="65"/>
       <c r="O23" s="65"/>
     </row>
-    <row r="24" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="65"/>
       <c r="B24" s="76" t="s">
         <v>53</v>
@@ -3434,7 +3450,7 @@
       <c r="N24" s="65"/>
       <c r="O24" s="65"/>
     </row>
-    <row r="25" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="65"/>
       <c r="B25" s="76" t="s">
         <v>54</v>
@@ -3453,7 +3469,7 @@
       <c r="N25" s="65"/>
       <c r="O25" s="65"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
       <c r="B26" s="62"/>
       <c r="C26" s="58"/>
@@ -3470,7 +3486,7 @@
       <c r="N26" s="54"/>
       <c r="O26" s="54"/>
     </row>
-    <row r="27" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="54"/>
       <c r="B27" s="63"/>
       <c r="C27" s="58"/>
@@ -3487,7 +3503,7 @@
       <c r="N27" s="80"/>
       <c r="O27" s="80"/>
     </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="54"/>
       <c r="B28" s="62"/>
       <c r="C28" s="58"/>
@@ -3507,7 +3523,7 @@
       <c r="O28" s="83"/>
       <c r="P28" s="79"/>
     </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="54"/>
       <c r="B29" s="54"/>
       <c r="C29" s="54"/>
@@ -3529,7 +3545,7 @@
       </c>
       <c r="P29" s="79"/>
     </row>
-    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="54"/>
       <c r="B30" s="54"/>
       <c r="C30" s="54"/>
@@ -3551,7 +3567,7 @@
       </c>
       <c r="P30" s="79"/>
     </row>
-    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="54"/>
       <c r="B31" s="54"/>
       <c r="C31" s="54"/>
@@ -3573,7 +3589,7 @@
       </c>
       <c r="P31" s="79"/>
     </row>
-    <row r="32" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="54"/>
       <c r="B32" s="54"/>
       <c r="C32" s="54"/>
@@ -3593,7 +3609,7 @@
       </c>
       <c r="P32" s="79"/>
     </row>
-    <row r="33" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N33" s="81"/>
       <c r="O33" s="81"/>
     </row>

</xml_diff>